<commit_message>
Added curve fits to Ch2-4 graphs.
</commit_message>
<xml_diff>
--- a/chapters/ch03-Population/datasets/PopulationCurveFit.xlsx
+++ b/chapters/ch03-Population/datasets/PopulationCurveFit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch03-Population/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60FB78B-7659-4640-93DF-EA5E4F71C371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606EFCA0-1A54-5E44-9FFB-9CFD83CB12EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -64,13 +64,16 @@
     <t>coeffs</t>
   </si>
   <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>r2</t>
   </si>
 </sst>
 </file>
@@ -6474,8 +6477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I71"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6512,7 +6515,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -6546,7 +6549,7 @@
         <v>2.6313571448151447</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K2" s="1">
         <v>2.555144161E-14</v>
@@ -6583,7 +6586,7 @@
         <v>2.6752589790216743</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" s="1">
         <v>1.654645251E-2</v>
@@ -6618,6 +6621,12 @@
       <c r="I4" s="1">
         <f t="shared" si="1"/>
         <v>2.7198932759615495</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.98914841939999998</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>